<commit_message>
added query feature for inventory and orders and refactored server.js code
</commit_message>
<xml_diff>
--- a/Homecoming.xlsx
+++ b/Homecoming.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -194,6 +194,60 @@
   </si>
   <si>
     <t>A18</t>
+  </si>
+  <si>
+    <t>coolio</t>
+  </si>
+  <si>
+    <t>meraj</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>fsfdsf</t>
+  </si>
+  <si>
+    <t>ahmeds85165@live.bucks.edu</t>
+  </si>
+  <si>
+    <t>technology committee</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>444</t>
+  </si>
+  <si>
+    <t>tech</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>cups</t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>A88</t>
+  </si>
+  <si>
+    <t>Cups</t>
   </si>
 </sst>
 </file>
@@ -545,7 +599,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="F4" sqref="F4"/>
@@ -1307,7 +1361,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>14</v>
       </c>
@@ -1328,6 +1382,167 @@
       </c>
       <c r="H21" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a download page with download buttons with routes, but still need actually make it so that the file will download
</commit_message>
<xml_diff>
--- a/Homecoming.xlsx
+++ b/Homecoming.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -599,7 +599,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="F4" sqref="F4"/>
@@ -1522,7 +1522,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>14</v>
       </c>
@@ -1543,6 +1543,29 @@
       </c>
       <c r="H28" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H29" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>